<commit_message>
Correction to demand data.
</commit_message>
<xml_diff>
--- a/ProductDemandComplete.xlsx
+++ b/ProductDemandComplete.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wjaarsveld\PycharmProjects\NatuurMedIntegration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E350511-E45F-4AE6-B933-57E066E504BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F969A6F6-6464-4E66-9C0A-4F4E52E857EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28615,7 +28615,7 @@
         <v>15</v>
       </c>
       <c r="F944">
-        <v>10000</v>
+        <v>10</v>
       </c>
       <c r="G944">
         <v>2</v>

</xml_diff>